<commit_message>
Fix print cheque decimal bug; Add ONLY when no cents
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/printCheque.xlsx
+++ b/src/main/resources/excel/printCheque.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -90,7 +90,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -98,6 +98,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -396,14 +399,14 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="2" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -441,7 +444,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="6">
+      <c r="H3" s="7">
         <v>9349.8700000000008</v>
       </c>
       <c r="I3" s="6"/>
@@ -516,7 +519,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0" bottom="0.75" header="0" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Adjust print cheque font size
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/printCheque.xlsx
+++ b/src/main/resources/excel/printCheque.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJ\git\magic\src\main\resources\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB187C17-A2FD-4DD1-9188-ED760137A86C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="72" windowWidth="20052" windowHeight="7932" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,11 +36,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +74,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -88,17 +100,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -108,6 +121,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -154,7 +175,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -186,9 +207,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -220,6 +259,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -395,22 +452,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" customWidth="1"/>
+    <col min="2" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -421,7 +478,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="21.95" customHeight="1">
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -429,14 +486,14 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" s="4" customFormat="1" ht="21.95" customHeight="1">
+    <row r="3" spans="1:9" s="4" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3"/>
@@ -444,14 +501,14 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="7">
+      <c r="H3" s="8">
         <v>9349.8700000000008</v>
       </c>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" s="5" customFormat="1" ht="21.95" customHeight="1">
+    <row r="4" spans="1:9" s="5" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="2"/>
@@ -462,7 +519,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -473,7 +530,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -484,7 +541,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -495,7 +552,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -506,7 +563,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -524,24 +581,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update print cheque excel
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/printCheque.xlsx
+++ b/src/main/resources/excel/printCheque.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJ\git\magic\src\main\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\IRENE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB187C17-A2FD-4DD1-9188-ED760137A86C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{42C72F97-A092-4D06-8554-BFBFCE1E451F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="72" windowWidth="20052" windowHeight="7932" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="13356" windowHeight="7776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,15 +22,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>WILKING GLOBAL, INC</t>
+    <t>SEPTEMBER 01, 2019</t>
   </si>
   <si>
-    <t>NINE THOUSAND THREE HUNDRED FORTY-NINE &amp; 87/100</t>
+    <t>EMPERADOR DISTILLERS, INC.</t>
   </si>
   <si>
-    <t>APRIL 22, 2017</t>
+    <t>227,900.00</t>
+  </si>
+  <si>
+    <t>TWO HUNDRED TWENTY-SEVEN THOUSAND NINE HUNDRED ONLY</t>
   </si>
 </sst>
 </file>
@@ -38,7 +41,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -100,7 +103,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -109,10 +112,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -456,15 +459,16 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" customWidth="1"/>
-    <col min="2" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.5546875" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1" collapsed="1"/>
+    <col min="2" max="6" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.21875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.5546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -478,7 +482,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -487,29 +491,29 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="7" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" s="4" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="4" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="8">
-        <v>9349.8700000000008</v>
+      <c r="H3" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" s="5" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="5" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="7" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -576,7 +580,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0" bottom="0.75" header="0" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>